<commit_message>
updated changes req on 28th
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\suji\SourceCode\SAP_Buildsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyindia-my.sharepoint.com/personal/suraj_acharya_in_ey_com/Documents/Desktop/Unilever/SAP_Buildsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FBA0FB-E923-45D2-9233-2329FD358A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{38202DA4-C953-4025-91E7-766F3A774A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9E22C21-6580-4CA8-B57A-7E7A9AA2F990}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E86B7F64-D4B2-42B2-BB21-CEFB44C19956}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E86B7F64-D4B2-42B2-BB21-CEFB44C19956}"/>
   </bookViews>
   <sheets>
     <sheet name="SAP" sheetId="3" r:id="rId1"/>
@@ -139,10 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
-  <si>
-    <t>op1x002a/op1x051a</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
   <si>
     <t>Allocation in GB</t>
   </si>
@@ -174,10 +171,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t xml:space="preserve">P1Xsaplocal
-</t>
-  </si>
-  <si>
     <t>usrsap</t>
   </si>
   <si>
@@ -190,34 +183,12 @@
     <t>No</t>
   </si>
   <si>
-    <t>P1Xsap</t>
-  </si>
-  <si>
-    <t>/usr/sap/P1X</t>
-  </si>
-  <si>
     <t>DAAsap</t>
   </si>
   <si>
     <t>/usr/sap/DAA</t>
   </si>
   <si>
-    <t>P1Xascs</t>
-  </si>
-  <si>
-    <t>/usr/sap/P1X/ASCS01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1XNFS
-</t>
-  </si>
-  <si>
-    <t>/srv/nfs/op1x</t>
-  </si>
-  <si>
-    <t>op1X002</t>
-  </si>
-  <si>
     <t>interface</t>
   </si>
   <si>
@@ -227,39 +198,9 @@
     <t>trans</t>
   </si>
   <si>
-    <t>&lt;NFS Server&gt;:/srv/nfs/op1x/interface</t>
-  </si>
-  <si>
-    <t>/interface/sapp1x</t>
-  </si>
-  <si>
-    <t>&lt;NFS Server&gt;:/srv/nfs/op1x/sapmnt</t>
-  </si>
-  <si>
-    <t>/sapmnt/P1X</t>
-  </si>
-  <si>
-    <t>&lt;NFS Server&gt;:/srv/nfs/op1x/op1x002</t>
-  </si>
-  <si>
-    <t>/app/op1x002</t>
-  </si>
-  <si>
-    <t>&lt;NFS Server&gt;:/srv/nfs/op1x/trans</t>
-  </si>
-  <si>
     <t>/usr/sap/trans</t>
   </si>
   <si>
-    <t>P1X Hana Standalone on Azure</t>
-  </si>
-  <si>
-    <t>P1X - System DB</t>
-  </si>
-  <si>
-    <t>P1X - Tenant DB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Node 1 </t>
   </si>
   <si>
@@ -281,34 +222,13 @@
     <t>Category</t>
   </si>
   <si>
-    <t>P1Xsaplocal</t>
-  </si>
-  <si>
     <t>/usr/sap/</t>
   </si>
   <si>
-    <t>P1Xhanashared</t>
-  </si>
-  <si>
-    <t>P1Xshared</t>
-  </si>
-  <si>
     <t>/hana/shared/</t>
   </si>
   <si>
-    <t>P1Xhanalog</t>
-  </si>
-  <si>
-    <t>P1Xlog</t>
-  </si>
-  <si>
     <t>/hana/log/</t>
-  </si>
-  <si>
-    <t>P1Xhanadata</t>
-  </si>
-  <si>
-    <t>P1Xdata</t>
   </si>
   <si>
     <t>/hana/data/</t>
@@ -523,8 +443,84 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">P1XNFS
+    <t xml:space="preserve">SIDsaplocal
 </t>
+  </si>
+  <si>
+    <t>SIDsap</t>
+  </si>
+  <si>
+    <t>/usr/sap/SID</t>
+  </si>
+  <si>
+    <t>SIDascs</t>
+  </si>
+  <si>
+    <t>/usr/sap/SID/ASCS01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIDNFS
+</t>
+  </si>
+  <si>
+    <t>/srv/nfs/oSID</t>
+  </si>
+  <si>
+    <t>oSID002</t>
+  </si>
+  <si>
+    <t>&lt;NFS Server&gt;:/srv/nfs/oSID/interface</t>
+  </si>
+  <si>
+    <t>/interface/sapSID</t>
+  </si>
+  <si>
+    <t>&lt;NFS Server&gt;:/srv/nfs/oSID/sapmnt</t>
+  </si>
+  <si>
+    <t>/sapmnt/SID</t>
+  </si>
+  <si>
+    <t>&lt;NFS Server&gt;:/srv/nfs/oSID/oSID002</t>
+  </si>
+  <si>
+    <t>/app/oSID002</t>
+  </si>
+  <si>
+    <t>&lt;NFS Server&gt;:/srv/nfs/oSID/trans</t>
+  </si>
+  <si>
+    <t>oSID002a/oSID051a</t>
+  </si>
+  <si>
+    <t>SID Hana Standalone on Azure</t>
+  </si>
+  <si>
+    <t>SID - System DB</t>
+  </si>
+  <si>
+    <t>SID - Tenant DB</t>
+  </si>
+  <si>
+    <t>SIDsaplocal</t>
+  </si>
+  <si>
+    <t>SIDhanashared</t>
+  </si>
+  <si>
+    <t>SIDshared</t>
+  </si>
+  <si>
+    <t>SIDhanalog</t>
+  </si>
+  <si>
+    <t>SIDlog</t>
+  </si>
+  <si>
+    <t>SIDhanadata</t>
+  </si>
+  <si>
+    <t>SIDdata</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1234,6 +1230,19 @@
     <xf numFmtId="0" fontId="22" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1261,17 +1270,50 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1291,64 +1333,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2503,8 +2487,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2597,10 +2581,10 @@
     <row r="2" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52"/>
       <c r="B2" s="52" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
@@ -2626,7 +2610,7 @@
       <c r="Y2" s="52"/>
       <c r="Z2" s="52"/>
       <c r="AA2" s="52" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="AB2" s="52"/>
       <c r="AC2" s="52"/>
@@ -2708,7 +2692,7 @@
       <c r="A4" s="52"/>
       <c r="B4" s="52"/>
       <c r="C4" s="52" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
@@ -2786,7 +2770,7 @@
       <c r="Y5" s="52"/>
       <c r="Z5" s="52"/>
       <c r="AA5" s="52" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="AB5" s="52"/>
       <c r="AC5" s="52"/>
@@ -2918,7 +2902,7 @@
     </row>
     <row r="8" spans="1:50" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="65" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B8" s="65"/>
       <c r="C8" s="65"/>
@@ -3001,184 +2985,184 @@
       <c r="AB9" s="53"/>
       <c r="AC9" s="53"/>
       <c r="AD9" s="68" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="AE9" s="69"/>
       <c r="AF9" s="68" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="AG9" s="69"/>
       <c r="AH9" s="68" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="AI9" s="69"/>
       <c r="AJ9" s="68" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="AK9" s="69"/>
       <c r="AL9" s="68" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="AM9" s="69"/>
       <c r="AN9" s="68" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="AO9" s="69"/>
       <c r="AP9" s="68" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="AQ9" s="69"/>
       <c r="AR9" s="63" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="AS9" s="63" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="AT9" s="63" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="AU9" s="63" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="AV9" s="63" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="AW9" s="66" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="AX9" s="63" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:50" ht="87" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="S10" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="U10" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="W10" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="X10" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y10" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z10" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA10" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB10" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC10" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD10" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="AE10" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="57" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="57" t="s">
-        <v>90</v>
-      </c>
-      <c r="K10" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="L10" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="M10" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="N10" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="O10" s="57" t="s">
-        <v>95</v>
-      </c>
-      <c r="P10" s="57" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q10" s="57" t="s">
-        <v>97</v>
-      </c>
-      <c r="R10" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="S10" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="T10" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="U10" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="V10" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="W10" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="X10" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y10" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z10" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA10" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB10" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC10" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD10" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE10" s="57" t="s">
-        <v>108</v>
-      </c>
       <c r="AF10" s="60" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="AG10" s="57" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="AH10" s="60" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="AI10" s="57" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="AJ10" s="60" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="AK10" s="57" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="AL10" s="60" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="AM10" s="57" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="AN10" s="60" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="AO10" s="57" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="AP10" s="60" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="AQ10" s="57" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="AR10" s="64"/>
       <c r="AS10" s="64"/>
@@ -3187,7 +3171,7 @@
       <c r="AV10" s="64"/>
       <c r="AW10" s="67"/>
       <c r="AX10" s="64" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
@@ -3844,14 +3828,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="36.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="9" customWidth="1"/>
@@ -3869,54 +3853,54 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="A2" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
     </row>
     <row r="3" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="73"/>
+      <c r="B4" s="77"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -3926,33 +3910,33 @@
       <c r="I4" s="15"/>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>5</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="E5" s="80"/>
+      <c r="F5" s="70">
+        <v>1</v>
+      </c>
+      <c r="G5" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="H5" s="78">
+        <v>128</v>
+      </c>
+      <c r="I5" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="79">
-        <v>1</v>
-      </c>
-      <c r="G5" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="74">
-        <v>128</v>
-      </c>
-      <c r="I5" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="74">
+      <c r="J5" s="78">
         <v>128</v>
       </c>
     </row>
@@ -3960,55 +3944,55 @@
       <c r="A6" s="17">
         <v>70</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="18" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
+        <v>89</v>
+      </c>
+      <c r="E6" s="81"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>20</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="77"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
+        <v>15</v>
+      </c>
+      <c r="E7" s="81"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>20</v>
       </c>
-      <c r="B8" s="103"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="18" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
+        <v>91</v>
+      </c>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
@@ -4022,77 +4006,79 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="82">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="71">
         <v>128</v>
       </c>
-      <c r="B10" s="102" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="106" t="s">
-        <v>23</v>
+      <c r="B10" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>93</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="79">
+        <v>94</v>
+      </c>
+      <c r="F10" s="70">
         <v>1</v>
       </c>
-      <c r="G10" s="79" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="79">
+      <c r="G10" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="70">
         <v>128</v>
       </c>
-      <c r="I10" s="79" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="79">
+      <c r="I10" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="70">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="23"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="71"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
-      <c r="C12" s="108"/>
-      <c r="D12" s="109"/>
+        <v>16</v>
+      </c>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="71"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
+        <v>17</v>
+      </c>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="71"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
+        <v>18</v>
+      </c>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
@@ -4108,12 +4094,12 @@
     </row>
     <row r="15" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="29"/>
       <c r="D15" s="28" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
@@ -4124,12 +4110,12 @@
     </row>
     <row r="16" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="29"/>
       <c r="D16" s="28" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
@@ -4140,12 +4126,12 @@
     </row>
     <row r="17" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
@@ -4156,12 +4142,12 @@
     </row>
     <row r="18" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
@@ -4171,21 +4157,25 @@
       <c r="J18" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G10:G13"/>
+  <mergeCells count="18">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="F5:F8"/>
     <mergeCell ref="G5:G8"/>
     <mergeCell ref="H5:H8"/>
     <mergeCell ref="I5:I8"/>
     <mergeCell ref="J5:J8"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -4197,13 +4187,13 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
@@ -4213,12 +4203,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="A1" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -4230,7 +4220,7 @@
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -4246,7 +4236,7 @@
     </row>
     <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -4261,74 +4251,74 @@
       <c r="L3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="86"/>
+      <c r="A4" s="99" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="101"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
+      <c r="A5" s="102"/>
       <c r="B5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="E5" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="87" t="s">
+      <c r="F5" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="72" t="s">
+      <c r="I5" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="89" t="s">
-        <v>10</v>
+      <c r="J5" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="85" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
+      <c r="A6" s="103"/>
       <c r="B6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
+        <v>25</v>
+      </c>
+      <c r="C6" s="77"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
       <c r="G6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="90"/>
+        <v>26</v>
+      </c>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="86"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
@@ -4347,73 +4337,73 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="40"/>
-      <c r="C8" s="99" t="s">
-        <v>46</v>
+      <c r="C8" s="87" t="s">
+        <v>106</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="96"/>
+        <v>27</v>
+      </c>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="95"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
       <c r="B9" s="40"/>
-      <c r="C9" s="100"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="38" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="97"/>
+        <v>89</v>
+      </c>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91"/>
+      <c r="L9" s="96"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="41"/>
       <c r="B10" s="40"/>
-      <c r="C10" s="101"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="38" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="93"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="98"/>
+        <v>15</v>
+      </c>
+      <c r="F10" s="92"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="92"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="97"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="41"/>
       <c r="B11" s="40"/>
       <c r="C11" s="42" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="F11" s="43"/>
-      <c r="G11" s="94"/>
+      <c r="G11" s="93"/>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
       <c r="J11" s="43"/>
@@ -4424,16 +4414,16 @@
       <c r="A12" s="41"/>
       <c r="B12" s="40"/>
       <c r="C12" s="45" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="F12" s="43"/>
-      <c r="G12" s="94"/>
+      <c r="G12" s="93"/>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
@@ -4444,16 +4434,16 @@
       <c r="A13" s="41"/>
       <c r="B13" s="40"/>
       <c r="C13" s="45" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F13" s="43"/>
-      <c r="G13" s="95"/>
+      <c r="G13" s="94"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
@@ -4467,7 +4457,7 @@
       <c r="D14" s="47"/>
       <c r="E14" s="47"/>
       <c r="F14" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -4482,7 +4472,7 @@
       <c r="C15" s="32"/>
       <c r="D15" s="1"/>
       <c r="E15" s="48" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F15" s="32">
         <f>SUM(F8:F14)</f>
@@ -4493,7 +4483,7 @@
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
       <c r="K15" s="32" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="L15" s="32">
         <f>SUM(L8:L14)</f>
@@ -4519,13 +4509,13 @@
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
       <c r="D17" s="50" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
@@ -4535,14 +4525,7 @@
       <c r="L17" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:I10"/>
+  <mergeCells count="20">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A5:A6"/>
@@ -4555,6 +4538,14 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="L8:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>